<commit_message>
version 5. se añaden los componentes correspondientes a los conectores interplaca.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\TEAMDR~1\JRODRI~1\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7C95B8-4A38-204A-83B9-B9BB0213CA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781D098C-8637-4042-92F9-09A2F430DB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="1100" windowWidth="23260" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="111">
   <si>
     <t>Qty</t>
   </si>
@@ -328,9 +328,6 @@
     <t>0R</t>
   </si>
   <si>
-    <t>5-ene-2023</t>
-  </si>
-  <si>
     <t>https://www.digikey.es/es/products/detail/nexperia-usa-inc/2N7002PW-115/2296328?s=N4IgTCBcDa4HYHYAMSwAcDuIC6BfIA</t>
   </si>
   <si>
@@ -353,6 +350,24 @@
   </si>
   <si>
     <t>https://www.digikey.es/es/products/detail/analog-devices-inc-maxim-integrated/MAX9062EUK-T/1937837</t>
+  </si>
+  <si>
+    <t>https://www.digikey.es/es/products/detail/hirose-electric-co-ltd/DF40C-2-0-20DS-0-4V-51/1967923</t>
+  </si>
+  <si>
+    <t>DF40C2020DS04V51</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>DF40C_2.0_-20DS-0.4V_51_</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Se añade la posicion 26</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1072,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1085,53 +1099,79 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -1181,31 +1221,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
@@ -1222,7 +1237,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H32" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H32" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A6:H32" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H32">
     <sortCondition ref="D6:D32"/>
@@ -1242,7 +1257,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1530,7 +1545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1538,61 +1553,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3">
         <f>MAX(_HISTORY!A4:A43)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
-      <c r="C4" s="21" t="s">
+    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+      <c r="C4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1618,7 +1633,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1644,7 +1659,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1690,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1736,7 +1751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1759,7 +1774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1782,7 +1797,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1808,7 +1823,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1831,10 +1846,10 @@
         <v>6</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1857,7 +1872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1880,7 +1895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1926,7 +1941,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -1960,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -1972,7 +1987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -1995,7 +2010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2006,13 +2021,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2058,7 +2073,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2084,7 +2099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2107,7 +2122,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2130,7 +2145,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2150,13 +2165,13 @@
         <v>20</v>
       </c>
       <c r="G29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2176,13 +2191,13 @@
         <v>20</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2203,20 +2218,46 @@
       </c>
       <c r="G31" s="10" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C4:F4"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B31">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="NO">
+  <conditionalFormatting sqref="B7:B32">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2227,34 +2268,35 @@
     <hyperlink ref="H15" r:id="rId4" xr:uid="{A55F8D7F-37A3-6F42-BF93-04D74AAFC390}"/>
     <hyperlink ref="H30" r:id="rId5" xr:uid="{A51211E8-ED6B-294D-9C2F-72984D2579E9}"/>
     <hyperlink ref="H29" r:id="rId6" xr:uid="{B325A5FF-4D2C-E84F-8774-9150BE2D1CE7}"/>
+    <hyperlink ref="H32" r:id="rId7" xr:uid="{8399F332-EFD1-4727-AC96-322D208DC5D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>71</v>
       </c>
@@ -2268,11 +2310,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="24">
         <v>44874</v>
       </c>
       <c r="C4" t="s">
@@ -2282,11 +2324,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="24">
         <v>44880</v>
       </c>
       <c r="C5" t="s">
@@ -2296,11 +2338,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="24">
         <v>44918</v>
       </c>
       <c r="C6" t="s">
@@ -2310,18 +2352,32 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>97</v>
+      <c r="B7" s="24">
+        <v>44931</v>
       </c>
       <c r="C7" t="s">
         <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="24">
+        <v>44958</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2337,72 +2393,72 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="B3" s="15"/>
+      <c r="C3" s="16"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>28805</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="20"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Se cambia el nombre de IC1 a U2 para  el supervisor de tension (conforme a PCB)
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAC93D5-3C6F-4242-A70C-AF1BC8B073DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA9819-57AD-E84B-82EC-0566094F2701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -367,9 +367,6 @@
     <t>R19,R48</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
     <t>MIC803-26D3VC3-TR</t>
   </si>
   <si>
@@ -414,6 +411,9 @@
 se crea la posicion 29 con el part R20
 Se crea la posicion 30 con el part R21
 La posicion 6 aumenta en 1 con el part C29</t>
+  </si>
+  <si>
+    <t>U2</t>
   </si>
 </sst>
 </file>
@@ -1134,6 +1134,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1146,131 +1149,53 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <border outline="0">
         <top style="thin">
@@ -1361,7 +1286,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H36" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H36" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A6:H36" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H32">
     <sortCondition ref="D6:D32"/>
@@ -1381,7 +1306,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1679,28 +1604,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1710,28 +1635,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
-      <c r="C4" s="21" t="s">
+    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+      <c r="C4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1757,7 +1682,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1783,7 +1708,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1806,7 +1731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1829,7 +1754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1852,7 +1777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1875,7 +1800,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1886,7 +1811,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E12" t="s">
         <v>90</v>
@@ -1898,7 +1823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1921,7 +1846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1947,7 +1872,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1973,7 +1898,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1996,7 +1921,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2019,7 +1944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -2042,7 +1967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -2065,7 +1990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2088,7 +2013,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2111,7 +2036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2134,7 +2059,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2151,7 +2076,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2174,7 +2099,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2197,7 +2122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2223,7 +2148,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2246,7 +2171,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2269,7 +2194,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2295,7 +2220,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2321,7 +2246,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2344,7 +2269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
@@ -2370,70 +2295,70 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="25">
+      <c r="C33" s="21">
         <v>1</v>
       </c>
       <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
         <v>110</v>
-      </c>
-      <c r="E33" t="s">
-        <v>111</v>
       </c>
       <c r="F33" t="s">
         <v>20</v>
       </c>
       <c r="G33" t="s">
+        <v>111</v>
+      </c>
+      <c r="H33" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="25">
+      <c r="C34" s="21">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F34" t="s">
         <v>21</v>
       </c>
       <c r="G34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="25">
+      <c r="C35" s="21">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" t="s">
         <v>94</v>
@@ -2442,30 +2367,30 @@
         <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="25">
+      <c r="C36" s="21">
         <v>1</v>
       </c>
       <c r="D36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E36" t="s">
         <v>118</v>
-      </c>
-      <c r="E36" t="s">
-        <v>119</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2473,13 +2398,13 @@
     <mergeCell ref="C4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B36">
-    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2510,17 +2435,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>70</v>
       </c>
@@ -2534,7 +2459,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2548,7 +2473,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2562,7 +2487,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2576,7 +2501,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2590,7 +2515,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2604,7 +2529,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2615,10 +2540,10 @@
         <v>74</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2629,7 +2554,7 @@
         <v>74</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2645,56 +2570,56 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>28805</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>83</v>
       </c>
@@ -2703,7 +2628,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Revisión BOM previa envio SETI
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0FAE46-D650-4C19-8A69-1D0BD2C0D50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A1C7F-291E-476B-8591-A35D05B07846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="123">
   <si>
     <t>Qty</t>
   </si>
@@ -356,15 +356,6 @@
   </si>
   <si>
     <t>Se añade la posicion 26</t>
-  </si>
-  <si>
-    <t>MIC803-26D3VC3-TR</t>
-  </si>
-  <si>
-    <t>SC70</t>
-  </si>
-  <si>
-    <t>https://www.digikey.es/es/products/detail/microchip-technology/MIC803-26D3VC3-TR/2566974</t>
   </si>
   <si>
     <t>C3, C5, C7, C9, C10, C11, C13, C15, C16, C17, C18, C19, C24, C25, C26, C27,C28,C29</t>
@@ -401,9 +392,6 @@
 La posicion 6 aumenta en 1 con el part C29</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>R4, R5, R14, R16</t>
   </si>
   <si>
@@ -418,6 +406,9 @@
   <si>
     <t>Se cambia el valor de R48 de 10k a 1k. Se decrementa en 1 la cantidad de la posicion 15 a 4  y se aumenta en una la posicion 16 a 3
 Se cambia el valor de R18 de 100k a 10k. Se crea la posicion 31 y se disminuye la poscion 16 a 2.</t>
+  </si>
+  <si>
+    <t>Se elimina el part U2 y por tanto, se elimina la posicion 27</t>
   </si>
 </sst>
 </file>
@@ -1141,6 +1132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1153,7 +1145,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,32 +1191,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1316,10 +1282,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H37" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}" name="Tabla1" displayName="Tabla1" ref="A6:H37" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A6:H37" xr:uid="{AD639D9D-BFED-4687-9866-69587ACF8311}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H32">
-    <sortCondition ref="D6:D32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:H37">
+    <sortCondition ref="A6:A37"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A4EEF5D5-EC32-4E92-A16D-A2C00D09EC58}" name="Position"/>
@@ -1635,7 +1601,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1628,7 @@
       <c r="B2" s="2"/>
       <c r="C2" s="3">
         <f>MAX(_HISTORY!A4:A43)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
@@ -1673,12 +1639,12 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="6"/>
@@ -1749,7 +1715,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
         <v>90</v>
@@ -1841,7 +1807,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E12" t="s">
         <v>89</v>
@@ -2054,7 +2020,7 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
@@ -2077,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E22" t="s">
         <v>24</v>
@@ -2097,7 +2063,7 @@
         <v>62</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>95</v>
@@ -2333,22 +2299,22 @@
         <v>63</v>
       </c>
       <c r="C33" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="F33" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>108</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>109</v>
+        <v>95</v>
+      </c>
+      <c r="H33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2362,10 +2328,10 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
         <v>21</v>
@@ -2374,7 +2340,7 @@
         <v>17</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2388,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E35" t="s">
         <v>93</v>
@@ -2411,10 +2377,10 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F36" t="s">
         <v>15</v>
@@ -2430,14 +2396,14 @@
       <c r="B37" t="s">
         <v>62</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="21">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E37" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F37" t="s">
         <v>15</v>
@@ -2451,13 +2417,13 @@
     <mergeCell ref="C4:F4"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:B37">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2469,7 +2435,7 @@
     <hyperlink ref="H30" r:id="rId5" xr:uid="{A51211E8-ED6B-294D-9C2F-72984D2579E9}"/>
     <hyperlink ref="H29" r:id="rId6" xr:uid="{B325A5FF-4D2C-E84F-8774-9150BE2D1CE7}"/>
     <hyperlink ref="H32" r:id="rId7" xr:uid="{8399F332-EFD1-4727-AC96-322D208DC5D3}"/>
-    <hyperlink ref="H33" r:id="rId8" xr:uid="{C62F63AE-5C2E-4B35-A8FC-B9620CDA7D2A}"/>
+    <hyperlink ref="H33" r:id="rId8" display="https://www.digikey.es/es/products/detail/microchip-technology/MIC803-26D3VC3-TR/2566974" xr:uid="{C62F63AE-5C2E-4B35-A8FC-B9620CDA7D2A}"/>
     <hyperlink ref="H34" r:id="rId9" xr:uid="{AB3206CD-2AFE-469F-80B6-B0657819E12B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2482,10 +2448,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,7 +2559,7 @@
         <v>73</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2607,21 +2573,35 @@
         <v>73</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="22">
         <v>45180</v>
       </c>
       <c r="C11" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="22">
+        <v>45194</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2640,11 +2620,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">

</xml_diff>

<commit_message>
Revision previa a envio SETI produccion 3
Se actualiza la columna de "NEW" que indica a SETI cambios en posiciones
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2A1C7F-291E-476B-8591-A35D05B07846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F865C664-9C96-D04B-9290-CCF6BB2B1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
   <si>
     <t>Qty</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>Se elimina el part U2 y por tanto, se elimina la posicion 27</t>
+  </si>
+  <si>
+    <t>Se actualiza la columna de NEW para que SETI tenga los cambios actualizados contra la version anterior (7)</t>
   </si>
 </sst>
 </file>
@@ -1147,49 +1150,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1302,7 +1305,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1600,28 +1603,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1631,14 +1634,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
@@ -1646,13 +1649,13 @@
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1704,12 +1707,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
@@ -1727,7 +1730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1796,12 +1799,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1">
         <v>18</v>
@@ -1819,7 +1822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1894,7 +1897,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2009,12 +2012,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -2032,7 +2035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2190,7 +2193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
@@ -2366,7 +2369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -2389,12 +2392,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C37" s="21">
         <v>1</v>
@@ -2448,23 +2451,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>69</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2548,7 +2551,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2576,7 +2579,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2590,7 +2593,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2602,6 +2605,17 @@
       </c>
       <c r="D12" s="11" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="22">
+        <v>45195</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2617,56 +2631,56 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>28805</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>82</v>
       </c>
@@ -2675,7 +2689,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Correccion error en celda de version
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F865C664-9C96-D04B-9290-CCF6BB2B1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DDF985-E6F1-4004-9A77-A32E2386CFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -1150,49 +1150,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1305,9 +1305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1345,7 +1345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1451,7 +1451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1593,7 +1593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1603,28 +1603,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1634,14 +1634,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
@@ -1649,13 +1649,13 @@
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>26</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
@@ -2453,21 +2453,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="135.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>69</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2607,7 +2607,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
       <c r="B13" s="22">
         <v>45195</v>
       </c>
@@ -2631,56 +2634,56 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>28805</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>82</v>
       </c>
@@ -2689,7 +2692,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Revert "Merge pull request #84 from MSTKMAD/develop"
This reverts commit 96fc117d3460fb5d771273194348358b85af1598, reversing
changes made to 9bb4215ab554844daf6eea25f914757804df500a.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DDF985-E6F1-4004-9A77-A32E2386CFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F865C664-9C96-D04B-9290-CCF6BB2B1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -1150,49 +1150,49 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1305,9 +1305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1345,7 +1345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1451,7 +1451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1593,7 +1593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1603,28 +1603,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1634,14 +1634,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
       <c r="C4" s="23" t="s">
         <v>22</v>
       </c>
@@ -1649,13 +1649,13 @@
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>12</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>13</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>14</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>21</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>23</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>24</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>25</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>26</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>27</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>28</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>29</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>30</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>31</v>
       </c>
@@ -2453,21 +2453,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>69</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2607,10 +2607,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="22">
         <v>45195</v>
       </c>
@@ -2634,56 +2631,56 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>78</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
         <v>28805</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>80</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>81</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>82</v>
       </c>
@@ -2692,7 +2689,7 @@
       </c>
       <c r="C8" s="19"/>
     </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Salto del compardor en arranques de alguna maquinas. #86
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER R-1/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER R-1/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\01.Rover\02.HARDWARE\V2-ROVER R-1\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F865C664-9C96-D04B-9290-CCF6BB2B1EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E156BA56-A77C-43E0-8B3A-450F2E8F7127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="125">
   <si>
     <t>Qty</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>R11</t>
-  </si>
-  <si>
-    <t>8k2</t>
   </si>
   <si>
     <t>U3</t>
@@ -412,6 +409,12 @@
   </si>
   <si>
     <t>Se actualiza la columna de NEW para que SETI tenga los cambios actualizados contra la version anterior (7)</t>
+  </si>
+  <si>
+    <t>11k</t>
+  </si>
+  <si>
+    <t>Se cambia el valor de R11 de 8k2 a 11k.</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1087,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1148,51 +1151,52 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1305,9 +1309,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1345,7 +1349,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1451,7 +1455,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1593,7 +1597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1603,70 +1607,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3">
         <f>MAX(_HISTORY!A4:A43)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="C4" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="24"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>1</v>
@@ -1678,254 +1682,254 @@
         <v>3</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1">
         <v>18</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
         <v>6</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
         <v>15</v>
       </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1934,16 +1938,16 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -1957,462 +1961,462 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
         <v>15</v>
       </c>
-      <c r="G18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
         <v>15</v>
       </c>
-      <c r="G20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
         <v>4</v>
       </c>
       <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
         <v>15</v>
       </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
         <v>15</v>
       </c>
-      <c r="G22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
         <v>15</v>
       </c>
-      <c r="G24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
         <v>15</v>
       </c>
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G29" t="s">
+        <v>98</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E31" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="G31" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="21">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="21">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="F34" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C35" s="21">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
         <v>15</v>
       </c>
-      <c r="G35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" s="21">
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
         <v>15</v>
       </c>
-      <c r="G36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C37" s="21">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
         <v>15</v>
-      </c>
-      <c r="G37" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2451,37 +2455,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="135.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="C3" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2489,13 +2493,13 @@
         <v>44874</v>
       </c>
       <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2503,13 +2507,13 @@
         <v>44880</v>
       </c>
       <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="D5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2517,13 +2521,13 @@
         <v>44918</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2531,13 +2535,13 @@
         <v>44931</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2545,13 +2549,13 @@
         <v>44958</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2559,13 +2563,13 @@
         <v>45062</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -2573,13 +2577,13 @@
         <v>45063</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -2587,13 +2591,13 @@
         <v>45180</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2601,21 +2605,35 @@
         <v>45194</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="22">
         <v>45195</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" s="27">
+        <v>45540</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2631,70 +2649,70 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
     </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
     </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>28805</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
     </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
     </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="C8" s="19"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="19"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="C9" s="16"/>
     </row>

</xml_diff>